<commit_message>
corrected results and WorldSmall2 results
</commit_message>
<xml_diff>
--- a/results/BrouerDesaulniersPisinger2014/CorrectionSheetResultsBrouerDesaulniersPisinger.xlsx
+++ b/results/BrouerDesaulniersPisinger2014/CorrectionSheetResultsBrouerDesaulniersPisinger.xlsx
@@ -5,17 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>InstanceName</t>
   </si>
@@ -33,6 +38,9 @@
   </si>
   <si>
     <t>Still Best</t>
+  </si>
+  <si>
+    <t>Solution with integer division corrected</t>
   </si>
   <si>
     <t>Baltic Low</t>
@@ -93,18 +101,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.00E+000"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,6 +136,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,7 +181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,7 +190,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -187,19 +202,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,21 +243,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="28.6632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,10 +268,10 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -260,332 +280,451 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <f aca="false">(1- 0.817857+2- 1.97798)*7*2.4*600*26</f>
         <v>53507.03904</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">-3.43424*10^6-C2</f>
         <v>-3487747.03904</v>
       </c>
+      <c r="G2" s="3" t="n">
+        <f aca="false">D2*(180/175)</f>
+        <v>-3587396.95444114</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">(1-0.817857)*7*2.4*600*26</f>
         <v>47736.03744</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">6.16513*10^6-C3</f>
         <v>6117393.96256</v>
       </c>
+      <c r="G3" s="3" t="n">
+        <f aca="false">D3*(180/175)</f>
+        <v>6292176.64720457</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <f aca="false">(2-1.97976)*7*2.4*600*26</f>
         <v>5304.49919999995</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <f aca="false">1.07648*10^7-C4</f>
         <v>10759495.5008</v>
       </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">D4*(180/175)</f>
+        <v>11066909.6579657</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <f aca="false">(2-1.80595)*7*2.4*600*26</f>
         <v>50856.624</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">1.14454*10^8-C5</f>
         <v>114403143.376</v>
       </c>
+      <c r="G5" s="3" t="n">
+        <f aca="false">D5*(180/175)</f>
+        <v>117671804.615314</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <f aca="false">(1-0.820238)*7*2.4*600*26</f>
         <v>47112.02496</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">1.3976*10^8-C6</f>
         <v>139712887.97504</v>
       </c>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
+      <c r="G6" s="3" t="n">
+        <f aca="false">D6*(180/175)</f>
+        <v>143704684.774327</v>
+      </c>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="n">
         <f aca="false">(3-2.88095)*7*2.4*600*26</f>
         <v>31200.6239999999</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">1.60611*10^8-C7</f>
         <v>160579799.376</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <v>156612000</v>
       </c>
-      <c r="F7" s="7" t="b">
-        <v>0</v>
+      <c r="F7" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">E7*(180/175)</f>
+        <v>161086628.571429</v>
+      </c>
+      <c r="H7" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="n">
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <f aca="false">-5.37*10^7</f>
         <v>-53700000</v>
       </c>
+      <c r="G8" s="3" t="n">
+        <f aca="false">D8*(180/175)</f>
+        <v>-55234285.7142857</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">(2-1.88452+1-0.927381)*7*2.4*600*26</f>
         <v>49296.98592</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="1" t="n">
         <f aca="false">-3.21529*10^7-C9</f>
         <v>-32202196.98592</v>
       </c>
+      <c r="G9" s="3" t="n">
+        <f aca="false">D9*(180/175)</f>
+        <v>-33122259.7569463</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <f aca="false">(1- 0.985714+2-1.89107+2-1.67857)*7*2.4*600*26</f>
         <v>116532.82368</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="1" t="n">
         <f aca="false">-2.3446*10^7-C10</f>
         <v>-23562532.82368</v>
       </c>
-    </row>
-    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5" t="n">
+      <c r="G10" s="3" t="n">
+        <f aca="false">D10*(180/175)</f>
+        <v>-24235748.0472137</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="n">
         <f aca="false">-6.48939*10^7</f>
         <v>-64893900</v>
       </c>
-      <c r="F11" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="n">
+      <c r="F11" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <f aca="false">D11*(180/175)</f>
+        <v>-66748011.4285714</v>
+      </c>
+      <c r="H11" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="5" t="n">
         <f aca="false">(2- 1.48095+1-0.855952)*7*2.4*600*26</f>
         <v>173784.72384</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="6" t="n">
         <f aca="false">6.97989*10^7-C12</f>
         <v>69625115.27616</v>
       </c>
-      <c r="E12" s="8" t="n">
+      <c r="E12" s="10" t="n">
         <v>76644600</v>
       </c>
-      <c r="F12" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5" t="n">
+      <c r="F12" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <f aca="false">E12*(180/175)</f>
+        <v>78834445.7142857</v>
+      </c>
+      <c r="H12" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="n">
         <f aca="false">1.57*10^8</f>
         <v>157000000</v>
       </c>
-      <c r="F13" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="n">
+      <c r="E13" s="0"/>
+      <c r="F13" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <f aca="false">D13*(180/175)</f>
+        <v>161485714.285714</v>
+      </c>
+      <c r="H13" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="n">
         <f aca="false">(1-0.667857)*7*2.4*600*26</f>
         <v>87048.03744</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="6" t="n">
         <f aca="false">8.62191*10^8-C14</f>
         <v>862103951.96256</v>
       </c>
-      <c r="E14" s="8" t="n">
+      <c r="E14" s="10" t="n">
         <v>912776000</v>
       </c>
-      <c r="F14" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5" t="n">
+      <c r="F14" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <f aca="false">E14*(180/175)</f>
+        <v>938855314.285714</v>
+      </c>
+      <c r="H14" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6" t="n">
         <f aca="false">1.40021*10^9</f>
         <v>1400210000</v>
       </c>
-      <c r="F15" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5" t="n">
+      <c r="E15" s="0"/>
+      <c r="F15" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <f aca="false">D15*(180/175)</f>
+        <v>1440216000</v>
+      </c>
+      <c r="H15" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6" t="n">
         <f aca="false">1.60076*10^9</f>
         <v>1600760000</v>
       </c>
-      <c r="F16" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5" t="n">
+      <c r="E16" s="0"/>
+      <c r="F16" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <f aca="false">D16*(180/175)</f>
+        <v>1646496000</v>
+      </c>
+      <c r="H16" s="9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6" t="n">
         <f aca="false">3.73*10^8</f>
         <v>373000000</v>
       </c>
-      <c r="F17" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3" t="n">
+      <c r="E17" s="0"/>
+      <c r="F17" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <f aca="false">D17*(180/175)</f>
+        <v>383657142.857143</v>
+      </c>
+      <c r="H17" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="4" t="n">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="n">
         <f aca="false">0.308336+(3-2.59286)*7*2.4*600*26</f>
         <v>106703.559536</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" s="6" t="n">
         <f aca="false">8.16971*10^8-C18</f>
         <v>816864296.440464</v>
       </c>
-      <c r="E18" s="6" t="n">
+      <c r="E18" s="7" t="n">
         <v>758549000</v>
       </c>
-      <c r="F18" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="3" t="n">
+      <c r="F18" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <f aca="false">E18*(180/175)</f>
+        <v>780221828.571429</v>
+      </c>
+      <c r="H18" s="9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C19" s="4" t="n">
+      <c r="C19" s="5" t="n">
         <f aca="false">(1-0.917857)*7*2.4*600+(2-1.79762)*7*2.4*600*26</f>
         <v>53867.75184</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="6" t="n">
         <f aca="false">1.01749*10^9-C19</f>
         <v>1017436132.24816</v>
       </c>
-      <c r="E19" s="6" t="n">
+      <c r="E19" s="7" t="n">
         <v>937461000</v>
       </c>
-      <c r="F19" s="7" t="b">
-        <v>1</v>
+      <c r="F19" s="8" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">E19*(180/175)</f>
+        <v>964245600</v>
+      </c>
+      <c r="H19" s="9" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>